<commit_message>
additional template documentation tweaks
</commit_message>
<xml_diff>
--- a/lib/inferno/apps/cli/templates/lib/%library_name%/requirements/Inferno Requirements Template.xlsx
+++ b/lib/inferno/apps/cli/templates/lib/%library_name%/requirements/Inferno Requirements Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/inferno-core/lib/inferno/apps/cli/templates/lib/%library_name%/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F74CE1-D794-4C47-8ABB-54FEA9834C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E9AA5-F00F-BA41-BC0A-C30DE28E9B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -89,21 +89,31 @@
         <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Purpose
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Extracting and Recording Requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-The primary purpose of this document is to help developers create the </t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Extracting requirements from an IG is a necessary step towards creating a complete test kit and enabling traceability between tests and the requirements they are testing.
+Extracting requirements from an IG is challenging. The requirements are often in a narrative context, use unclear language, and do not have an associated identifier. Details on breaking up compound requirements and clarifying the language for a requirement is included in </t>
     </r>
     <r>
       <rPr>
@@ -113,118 +123,16 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Requirements List CSV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Out-of-Scope Requirements List CSV </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">documents. The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Requirements CSV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is the authoritative source for  requirements extracted from an Implementation Guide. The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Out-of-Scope Requirements List CSV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> defines which requirements will not be tested in Inferno.
-These two files will be combined with annotations within Inferno test kits indicating which tests verify which requirements to generate a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Requirement Coverage Matrix CSV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> that details which requirements are verified and where work is still needed.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Filename and Requirement Set ID
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-This document will be named using an official identifier for the requirement set (Requirement Set Id) with the suffix "_reqs".
-To find the Requirement Set Id for an IG, scroll to the footer on the IG page and copy the identifier that looks like "hl7.fhir.us.davinci-drug-formulary#2.0.1". Then, replace the "#" with an underscore.
-For example, the Requirement Set Id name for  the Da Vinci Drug Formulary v2.0.1 would be  "hl7.fhir.us.davinci-drug-formulary_2.0.1" and the excel file name would be "hl7.fhir.us.davinci-drug-formulary_2.0.1_reqs.xslx". 
-This requirement set will also be used as the namespace for referencing requirements from this document and will be defined in the Metadata tab under "Id"</t>
+      <t>Further Considerations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> below.</t>
     </r>
   </si>
   <si>
@@ -235,607 +143,6 @@
         <color theme="1"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t>Exporting to CSVs</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To export data from this sheet into the Requirements List CSV  and Out-of-Scope Requirements List CSV files, follow the instructions in the "</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Converting the template to source-controlled artifacts</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" section of the Requirements and Traceability guide located here: https://mitre.sharepoint.com/:f:/r/sites/Inferno/Shared%20Documents/Testing%20and%20Development/Requirements%20Gathering?csf=1&amp;web=1&amp;e=8aTIeB
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>Extracting and Recording Requirements</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Extracting requirements from an IG is a necessary step towards creating a complete test kit and enabling traceability between tests and the requirements they are testing.
-Extracting requirements from an IG is challenging. The requirements are often in a narrative context, use unclear language, and do not have an associated identifier. Details on breaking up compound requirements and clarifying the language for a requirement is included in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Further Considerations</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> below.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Exported Columns
-Columns that get exported to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Requirements List CSV </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>file are yellow. Many of these values map to elements within the R5 Requirements element. Columns that get exported into the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Out-of-Scope Requirements List CSV </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> file are orange. Do not remove, rename, or reorder these columns.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Required Columns
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Required columns are denoted with an `*` in the column name.
-You must populate required columns.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ID*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The unique identifier for the requirement. IDs are short, meaningless (they do not contain context like section numbers), and numeric. An approach is incrementing integers. See below for how to handle IDs for child requirements.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: ID -&gt; Requirements.statement.key
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">URL*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The URL of the deepest section that contains the requirement. The URL provides context for the requirement text.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: URL -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Requirements.statement.reference
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Requirement*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A direct quote from the IG. Add any clarifications or interpretations in a helper column like the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test Plan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column. May include helpful context in square brackets.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Requirement -&gt; Requirements.statement.requirement
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Conformance*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The conformance verb of the requirement: SHALL, SHOULD, MAY, SHOULD NOT, SHALL NOT and DEPRECATED (see </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Further Consideration</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> below for when to use DEPRECATED).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Conformance -&gt; Requirements.statement.conformance
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Actors*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The actor, or actors, that the requirement constrains. The values will depend on the target specification, e.g., for Subscriptions (https://hl7.org/fhir/uv/subscriptions-backport/STU1.1/actors.html), Client and Server.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Actor -&gt; Requirements.actor
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Sub-requirement(s)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The requirement set id and requirement id(s) of external requirements that are referenced by this requirement. This column will only be used when this requirements document points to requirements from a different requirement set.  For example, PDex references US Core. When creating the requirements for the PDex test kit, the US Core requirement set id will be noted in this column for the PDex requirement(s) that reference US Core.
-Format: &lt;requirement set id&gt;@&lt;list of requirement ids and ranges&gt;. E.g., the requirement set with id "hl7.fhir.us.davinci-drug-formulary_2.0.1" and requirement id "40", "41", "42", and "50"  would get referenced by "hl7.fhir.us.davinci-drug-formulary_2.0.1@40-42,50"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Sub-requirements -&gt; Requirements.statement.parent
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Conditionality
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Whether or not the requirement is conditional on a prerequisite clause. An example of a conditional requirement is, "If the value is X, then the server SHALL do Y." Note: A blank value carries no information and does not indicate if </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Conditionality</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is true or false.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Conditionality -&gt; Requirements.statement.conditionality.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Verifiable?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A determination as to whether this requirement can be verified:: 'No' - the requirement cannot be verified, e.g., because it is not specific enough; 'Yes' - the requirement can be verified using mechanical means or an attestation.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Verifiability Details
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Details explaining the answer in the Verifiable? column, typically providing a rationale for why a given requirement will not be tested.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Planning To Test?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A determination as to whether this requirement will be tested. It might not be tested because it conflicts with another requirement or because it is a MAY requirement without any sub requirements.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Planning To Test Details
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Details explaining the answer in the Planning To Test? column, typically providing a rationale for why a given requirement will not be tested.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mapping: none</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
       <t>Auto-Generated Columns</t>
     </r>
     <r>
@@ -920,185 +227,6 @@
       <t xml:space="preserve">
 The section the requirement came from, extracted from the URL.
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>Helper Columns</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Helper columns are green and are meant to help you, the developer, write tests that align to the requirements. Modify, ignore, or delete as needed
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Conditionality Description
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">If the requirement is conditional, detail on when it is in force.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Section #
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Section number for the section of the IG the requirement comes from. Can be helpful for sorting and putting related / close-by sections together.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Group
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Any label you like to help organize the requirements to make test development easier.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Priority
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The relative priority of testing this requirement versus the other requirements. Helpful for determining what requirement tests to drop if time constraints become an issue.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Test Plan
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A high level outline of how Inferno will test the requirement.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Questions
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Any questions you have about the requirement.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Notes
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Miscellaneous details without another place (e.g., why a requirement was deprecated)</t>
     </r>
   </si>
   <si>
@@ -1624,12 +752,739 @@
       <t>E.g., for  Da Vinci Payer Data Exchange (v2.0.0: STU2), Reference would be https://hl7.org/fhir/us/davinci-pdex/STU2/.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Purpose
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The primary purpose of this document is to help developers document discrete requirements extracted from narrative sections of FHIR IGs and related regulations. A subset of the information in it will be extracted for use within Inferno for the tracking and display of requirements. Other fields are meant to assist in planning and implementation as well as understanding decisions that were made during extraction.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Filename and Requirement Set ID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+This should be named in a way that makes clear the requirement set that it contains the requirements for. The formal id of the requirement set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>must</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> be entered on the Metadata tab.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Exported Columns
+Columns that get exported to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Requirements List CSV </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">file are yellow. Many of these values map to elements within the R5 Requirements element.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Required Columns
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Required columns are denoted with an `*` in the column name.
+You must populate required columns.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Helper Columns</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Helper columns are green and are meant to help you, the developer, write tests that align to the requirements. Modify, ignore, or delete as needed
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Conditionality Description
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">If the requirement is conditional, detail on when it is in force.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Section #
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Section number for the section of the IG the requirement comes from. Can be helpful for sorting and putting related / close-by sections together.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Group
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Any label you like to help organize the requirements to make test development easier.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Priority
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The relative priority of testing this requirement versus the other requirements. Helpful for determining what requirement tests to drop if time constraints become an issue.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Test Plan
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A high level outline of how Inferno will test the requirement.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Questions
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Any questions you have about the requirement.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Notes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Miscellaneous details without another place, including breadcrubs regarding why a decision was made (e.g., why a requirement was deprecated, or why a certain conformance verb was chosen)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Exporting to CSVs</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To export data from this sheet into the Requirements CSV file, use the requirements export_csv script defined in the Inferno CLI (see https://inferno-framework.github.io/docs/advanced-test-features/requirements for details)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ID*
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The unique identifier for the requirement. If the source defines specific Ids for its requirement and they are at the right level of granulairty,they may be used. Otherwise generate ID values for each requirement, typically as short, meaningless (they do not contain context like section numbers), numeric identifiers. One approach is incrementing integers.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: ID -&gt; Requirements.statement.key
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">URL*
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The URL of the deepest section that contains the requirement. The URL provides context for the requirement text.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: URL -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Requirements.statement.reference
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Requirement*
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A direct quote from the IG, with additional context needed to make it stand-alone added in square brackets. An ellipsis should be used when omiting content.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: Requirement -&gt; Requirements.statement.requirement
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Conformance*
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The conformance verb of the requirement: SHALL, SHOULD, MAY, SHOULD NOT, SHALL NOT and DEPRECATED (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Further Consideration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> below for when to use DEPRECATED).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: Conformance -&gt; Requirements.statement.conformance
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Actors*
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The actor, or actors, that the requirement constrains. The values will depend on the target specification, e.g., for Subscriptions (https://hl7.org/fhir/uv/subscriptions-backport/STU1.1/actors.html), Client and Server.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: Actor -&gt; Requirements.actor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sub-requirement(s)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The requirement set id and requirement id(s) of external requirements that are referenced by this requirement. This column will only be used when this requirements document points to requirements from a different requirement set.  For example, PDex references US Core. When creating the requirements for the PDex test kit, the US Core requirement set id will be noted in this column for the PDex requirement(s) that reference US Core.
+Format: &lt;requirement set id&gt;@&lt;list of requirement ids and ranges&gt;. E.g., the requirement set with id "hl7.fhir.us.davinci-drug-formulary_2.0.1" and requirement id "40", "41", "42", and "50"  would get referenced by "hl7.fhir.us.davinci-drug-formulary_2.0.1@40-42,50". Or &lt;requirement set id&gt;#&lt;actor&gt; to reference all requirements from a requirements set for a particular actor.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: Sub-requirements -&gt; Requirements.statement.parent
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Conditionality
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Whether or not the requirement is conditional on a prerequisite clause. An example of a conditional requirement is, "If the value is X, then the server SHALL do Y." Note: A blank value carries no information and does not indicate if </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Conditionality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is true or false.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: Conditionality -&gt; Requirements.statement.conditionality.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Verifiable?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A determination as to whether this requirement can be verified:: 'No' - the requirement cannot be verified, e.g., because it is not specific enough; 'Yes' - the requirement can be verified using mechanical means or an attestation.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Verifiability Details
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Details explaining the answer in the Verifiable? column, typically providing a rationale for why a given requirement will not be tested.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Planning To Test?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A determination as to whether this requirement will be tested by any test kit. It might not be tested because it conflicts with another requirement or because it is a MAY requirement without any sub requirements.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mapping: none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Planning To Test Details
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Details explaining the answer in the Planning To Test? column, typically providing a rationale for why a given requirement will not be tested.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mapping: none</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1754,15 +1609,8 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1811,20 +1659,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1921,19 +1757,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="1"/>
       </left>
       <right/>
@@ -1988,7 +1811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2055,33 +1878,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2095,7 +1908,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2438,8 +2251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AA7094-ECFF-0B4E-A5C9-6F41B8D76EEB}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2452,60 +2265,60 @@
   <sheetData>
     <row r="1" spans="1:3" ht="340" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="39"/>
+        <v>0</v>
+      </c>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:3" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="36"/>
+        <v>61</v>
+      </c>
+      <c r="C3" s="33"/>
     </row>
     <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="33"/>
     </row>
     <row r="6" spans="1:3" ht="164" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="28"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="45"/>
+      <c r="A7" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="41"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="46"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="42"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
-      <c r="B9" s="40"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="37"/>
     </row>
     <row r="10" spans="1:3" ht="292" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2526,7 +2339,7 @@
   <dimension ref="A1:AJ348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2538,10 +2351,10 @@
     <col min="6" max="6" width="13.33203125" style="8" customWidth="1"/>
     <col min="7" max="7" width="14" style="7" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10" style="32" customWidth="1"/>
-    <col min="10" max="10" width="22" style="32" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="32" customWidth="1"/>
-    <col min="12" max="12" width="25.83203125" style="32" customWidth="1"/>
+    <col min="9" max="9" width="10" style="8" customWidth="1"/>
+    <col min="10" max="10" width="22" style="8" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="8" customWidth="1"/>
+    <col min="12" max="12" width="25.83203125" style="8" customWidth="1"/>
     <col min="13" max="13" width="20" style="9" customWidth="1"/>
     <col min="14" max="14" width="28.5" style="9" customWidth="1"/>
     <col min="15" max="16" width="10.83203125" style="10"/>
@@ -2557,64 +2370,64 @@
   <sheetData>
     <row r="1" spans="1:36" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="O1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="P1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="Q1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="U1" s="6"/>
       <c r="Z1" s="6"/>
@@ -2624,33 +2437,33 @@
         <v>12</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G2" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>35</v>
+      <c r="I2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="M2" s="9" t="str" cm="1">
         <f t="array" ref="M2">PAGE_NAME(B2)</f>
@@ -2680,10 +2493,10 @@
       <c r="F3" s="8"/>
       <c r="G3" s="7"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
       <c r="M3" s="9" t="str" cm="1">
         <f t="array" ref="M3">PAGE_NAME(B3)</f>
         <v/>
@@ -3927,10 +3740,10 @@
       </c>
     </row>
     <row r="122" spans="9:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="I122" s="33"/>
-      <c r="J122" s="33"/>
-      <c r="K122" s="33"/>
-      <c r="L122" s="33"/>
+      <c r="I122" s="7"/>
+      <c r="J122" s="7"/>
+      <c r="K122" s="7"/>
+      <c r="L122" s="7"/>
       <c r="M122" s="9" t="str" cm="1">
         <f t="array" ref="M122">PAGE_NAME(B122)</f>
         <v/>
@@ -6255,7 +6068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
@@ -6266,68 +6079,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="47"/>
+      <c r="A1" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="43"/>
     </row>
     <row r="2" spans="1:2" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -6354,19 +6167,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -6374,13 +6187,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -6400,67 +6213,67 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -6469,6 +6282,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -6722,29 +6557,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E19681A-8DD3-40CB-9262-8533E89B98A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6762,23 +6594,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
clean up info sheet
</commit_message>
<xml_diff>
--- a/lib/inferno/apps/cli/templates/lib/%library_name%/requirements/Inferno Requirements Template.xlsx
+++ b/lib/inferno/apps/cli/templates/lib/%library_name%/requirements/Inferno Requirements Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/inferno-core/lib/inferno/apps/cli/templates/lib/%library_name%/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E9AA5-F00F-BA41-BC0A-C30DE28E9B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027030A2-86B7-144D-82D2-9BC5810EC972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -82,259 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>Extracting and Recording Requirements</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Extracting requirements from an IG is a necessary step towards creating a complete test kit and enabling traceability between tests and the requirements they are testing.
-Extracting requirements from an IG is challenging. The requirements are often in a narrative context, use unclear language, and do not have an associated identifier. Details on breaking up compound requirements and clarifying the language for a requirement is included in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Further Considerations</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> below.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>Auto-Generated Columns</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Auto-Generated columns are blue.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Auto-Generated columns are populated based on information from the required columns.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Page</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-The page the requirement came from, extracted from the URL.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Section</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-The section the requirement came from, extracted from the URL.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>Further considerations</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>How to handle compound requirements</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Many statements in IGs are compound requirements: they contain multiple requirements in a single context.
-Below is an example of splitting up a compound requirement:
-Original text: The ice cream parlor SHALL sell ice cream in waffle cones and offer chocolate sprinkle toppings.
-Requirements:
-1. The ice cream parlor SHALL sell icecream in waffle cones.
-2. The ice cream parlor SHALL... offer chocolate sprinkle toppings.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">How to handle removing a requirement
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">If after release of the requirements artifact, if a requirement must be removed for some reason, its ID must be retired. To remove a requirement and indicate that the ID is retired, set the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Conformance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> column to DEPRECATED. Note that release may include the start of development of a test kit where requirement IDs have been mapped to tests as ensuring they are up to date with respect to the new requirement Ids may be tricky.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOTE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> This is only necessary after release / use of the IDs within a test kit. Feel free to remove requirements, change IDs, etc., prior to this point.</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
   <si>
     <t>ID*</t>
   </si>
@@ -753,73 +501,52 @@
     </r>
   </si>
   <si>
+    <t>The primary purpose of this document is to help developers document discrete requirements extracted from narrative sections of FHIR IGs and related regulations. A subset of the information in it will be extracted for use within Inferno for the tracking and display of requirements within Inferno. Other fields are meant to assist in planning and implementation as well as understanding decisions that were made during extraction.</t>
+  </si>
+  <si>
+    <t>Usage By Inferno</t>
+  </si>
+  <si>
+    <t>Why Extract Requirements</t>
+  </si>
+  <si>
+    <t>How to Extract Requirements</t>
+  </si>
+  <si>
+    <t>Extracting requirements from an IG is a helpful step towards creating a complete test kit, enabling the extracted requirements to be associated with suites and tests to enable traceability of which requirements are tested and where and which are not yet verified.</t>
+  </si>
+  <si>
+    <t>This spreadsheet is not used directly by Inferno. Requirements from it must be exported to a similar CSV form. To export data from this sheet into the Requirements CSV file, use the requirements export_csv command defined in the Inferno CLI (see https://inferno-framework.github.io/docs/advanced-test-features/requirements for details).
+- For the export_csv command to work, the formal id of the requirement set must be entered on the Metadata tab.
+- Inferno places no requirements on the filename, but this file should be named in a way that makes clear the requirement set that it contains the requirements for.</t>
+  </si>
+  <si>
+    <t>General Information</t>
+  </si>
+  <si>
+    <t>Exported Columns</t>
+  </si>
+  <si>
+    <t>Column Details</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section describes the columns on the Requirements sheet that are used to record information about an individual </t>
+  </si>
+  <si>
+    <t>Column Types</t>
+  </si>
+  <si>
+    <t>Required Columns</t>
+  </si>
+  <si>
+    <t>Required columns are denoted with an `*` in the column name. Required columns must be populated. If a required column is not populated for a requirement, Inferno may not load or use the requirement correctly.</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Purpose
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-The primary purpose of this document is to help developers document discrete requirements extracted from narrative sections of FHIR IGs and related regulations. A subset of the information in it will be extracted for use within Inferno for the tracking and display of requirements. Other fields are meant to assist in planning and implementation as well as understanding decisions that were made during extraction.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Filename and Requirement Set ID
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-This should be named in a way that makes clear the requirement set that it contains the requirements for. The formal id of the requirement set </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> be entered on the Metadata tab.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Exported Columns
-Columns that get exported to the </t>
+      <t xml:space="preserve">Columns that get exported to the </t>
     </r>
     <r>
       <rPr>
@@ -838,653 +565,167 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">file are yellow. Many of these values map to elements within the R5 Requirements element.
-</t>
+      <t>file are highlighted in yellow. Many of these values map to elements within the R5 Requirements element (see details in the column details section).</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Required Columns
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Required columns are denoted with an `*` in the column name.
-You must populate required columns.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>Helper Columns</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Helper columns are green and are meant to help you, the developer, write tests that align to the requirements. Modify, ignore, or delete as needed
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Conditionality Description
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">If the requirement is conditional, detail on when it is in force.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Section #
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Section number for the section of the IG the requirement comes from. Can be helpful for sorting and putting related / close-by sections together.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Group
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Any label you like to help organize the requirements to make test development easier.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Priority
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The relative priority of testing this requirement versus the other requirements. Helpful for determining what requirement tests to drop if time constraints become an issue.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Test Plan
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A high level outline of how Inferno will test the requirement.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Questions
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Any questions you have about the requirement.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Notes
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Miscellaneous details without another place, including breadcrubs regarding why a decision was made (e.g., why a requirement was deprecated, or why a certain conformance verb was chosen)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>Exporting to CSVs</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To export data from this sheet into the Requirements CSV file, use the requirements export_csv script defined in the Inferno CLI (see https://inferno-framework.github.io/docs/advanced-test-features/requirements for details)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ID*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The unique identifier for the requirement. If the source defines specific Ids for its requirement and they are at the right level of granulairty,they may be used. Otherwise generate ID values for each requirement, typically as short, meaningless (they do not contain context like section numbers), numeric identifiers. One approach is incrementing integers.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: ID -&gt; Requirements.statement.key
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">URL*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The URL of the deepest section that contains the requirement. The URL provides context for the requirement text.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: URL -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Requirements.statement.reference
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Requirement*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A direct quote from the IG, with additional context needed to make it stand-alone added in square brackets. An ellipsis should be used when omiting content.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Requirement -&gt; Requirements.statement.requirement
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Conformance*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The conformance verb of the requirement: SHALL, SHOULD, MAY, SHOULD NOT, SHALL NOT and DEPRECATED (see </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Further Consideration</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> below for when to use DEPRECATED).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Conformance -&gt; Requirements.statement.conformance
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Actors*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The actor, or actors, that the requirement constrains. The values will depend on the target specification, e.g., for Subscriptions (https://hl7.org/fhir/uv/subscriptions-backport/STU1.1/actors.html), Client and Server.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Actor -&gt; Requirements.actor
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Sub-requirement(s)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The requirement set id and requirement id(s) of external requirements that are referenced by this requirement. This column will only be used when this requirements document points to requirements from a different requirement set.  For example, PDex references US Core. When creating the requirements for the PDex test kit, the US Core requirement set id will be noted in this column for the PDex requirement(s) that reference US Core.
-Format: &lt;requirement set id&gt;@&lt;list of requirement ids and ranges&gt;. E.g., the requirement set with id "hl7.fhir.us.davinci-drug-formulary_2.0.1" and requirement id "40", "41", "42", and "50"  would get referenced by "hl7.fhir.us.davinci-drug-formulary_2.0.1@40-42,50". Or &lt;requirement set id&gt;#&lt;actor&gt; to reference all requirements from a requirements set for a particular actor.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Sub-requirements -&gt; Requirements.statement.parent
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Conditionality
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Whether or not the requirement is conditional on a prerequisite clause. An example of a conditional requirement is, "If the value is X, then the server SHALL do Y." Note: A blank value carries no information and does not indicate if </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Conditionality</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is true or false.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: Conditionality -&gt; Requirements.statement.conditionality.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Verifiable?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A determination as to whether this requirement can be verified:: 'No' - the requirement cannot be verified, e.g., because it is not specific enough; 'Yes' - the requirement can be verified using mechanical means or an attestation.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Verifiability Details
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Details explaining the answer in the Verifiable? column, typically providing a rationale for why a given requirement will not be tested.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Planning To Test?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A determination as to whether this requirement will be tested by any test kit. It might not be tested because it conflicts with another requirement or because it is a MAY requirement without any sub requirements.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mapping: none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Planning To Test Details
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Details explaining the answer in the Planning To Test? column, typically providing a rationale for why a given requirement will not be tested.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mapping: none</t>
-    </r>
+  </si>
+  <si>
+    <t>Helper Columns</t>
+  </si>
+  <si>
+    <t>Auto-Generated columns are highlighed in blue. Auto-Generated columns are populated based on information from the required columns.</t>
+  </si>
+  <si>
+    <t>Auto-Generated Columns</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>R5 Requirements Mapping</t>
+  </si>
+  <si>
+    <t>The unique identifier for the requirement. If the source defines specific Ids for its requirement and they are at the right level of granulairty,they may be used. Otherwise generate ID values for each requirement, typically as short, meaningless (they do not contain context like section numbers), numeric identifiers. One approach is to use incrementing integers.</t>
+  </si>
+  <si>
+    <t>Requirements.statement.key</t>
+  </si>
+  <si>
+    <t>The URL of the deepest section that contains the requirement. The URL provides context for the requirement text.</t>
+  </si>
+  <si>
+    <t>Requirements.statement.reference</t>
+  </si>
+  <si>
+    <t>A direct quote from the IG, with additional context needed to make it stand-alone added in square brackets. An ellipsis should be used when omiting content.</t>
+  </si>
+  <si>
+    <t>Requirements.statement.requirement</t>
+  </si>
+  <si>
+    <t>The conformance verb of the requirement: SHALL, SHOULD, MAY, SHOULD NOT, SHALL NOT and DEPRECATED (see Further Consideration below for when to use DEPRECATED).</t>
+  </si>
+  <si>
+    <t>Requirements.statement.conformance</t>
+  </si>
+  <si>
+    <t>The actor, or actors, that the requirement constrains. The values will depend on the target specification, e.g., for Subscriptions (https://hl7.org/fhir/uv/subscriptions-backport/STU1.1/actors.html), Client and Server.</t>
+  </si>
+  <si>
+    <t>Requirements.actor</t>
+  </si>
+  <si>
+    <t>Sub-requirement(s)</t>
+  </si>
+  <si>
+    <t>The requirement set id and requirement id(s) of external requirements that are referenced by this requirement. This column will only be used when this requirements document points to requirements from a different requirement set.  For example, PDex references US Core. When creating the requirements for the PDex test kit, the US Core requirement set id will be noted in this column for the PDex requirement(s) that reference US Core.
+Format: &lt;requirement set id&gt;@&lt;list of requirement ids and ranges&gt;. E.g., the requirement set with id "hl7.fhir.us.davinci-drug-formulary_2.0.1" and requirement id "40", "41", "42", and "50"  would get referenced by "hl7.fhir.us.davinci-drug-formulary_2.0.1@40-42,50". Or &lt;requirement set id&gt;#&lt;actor&gt; to reference all requirements from a requirements set for a particular actor.</t>
+  </si>
+  <si>
+    <t>Requirements.statement.parent</t>
+  </si>
+  <si>
+    <t>Whether or not the requirement is conditional on a prerequisite clause. An example of a conditional requirement is, "If the value is X, then the server SHALL do Y." Note: A blank value carries no information and does not indicate if Conditionality is true or false.</t>
+  </si>
+  <si>
+    <t>Requirements.statement.conditionality</t>
+  </si>
+  <si>
+    <t>A determination as to whether this requirement can be verified:: 'No' - the requirement cannot be verified, e.g., because it is not specific enough; 'Yes' - the requirement can be verified using mechanical means or an attestation.</t>
+  </si>
+  <si>
+    <t>Details explaining the answer in the Verifiable? column, typically providing a rationale for why a given requirement will not be tested.</t>
+  </si>
+  <si>
+    <t>A determination as to whether this requirement will be tested by any test kit. It might not be tested because it conflicts with another requirement or because it is a MAY requirement without any sub requirements.</t>
+  </si>
+  <si>
+    <t>Details explaining the answer in the Planning To Test? column, typically providing a rationale for why a given requirement will not be tested.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>The page the requirement came from, extracted from the URL.</t>
+  </si>
+  <si>
+    <t>The section the requirement came from, extracted from the URL.</t>
+  </si>
+  <si>
+    <t>Conditionality Description</t>
+  </si>
+  <si>
+    <t>If the requirement is conditional, detail on when it is in force.</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Section number for the section of the IG the requirement comes from. Can be helpful for sorting and putting related / close-by sections together.</t>
+  </si>
+  <si>
+    <t>Any label you like to help organize the requirements to make test development easier.</t>
+  </si>
+  <si>
+    <t>The relative priority of testing this requirement versus the other requirements. Helpful for determining what requirement tests to drop if time constraints become an issue.</t>
+  </si>
+  <si>
+    <t>A high level outline of how Inferno will test the requirement.</t>
+  </si>
+  <si>
+    <t>Any questions you have about the requirement. Can potentially be used to bring feedback to the IG authors.</t>
+  </si>
+  <si>
+    <t>Miscellaneous details without another place, including breadcrubs regarding why a decision was made (e.g., why a requirement was deprecated, or why a certain conformance verb was chosen).</t>
+  </si>
+  <si>
+    <t>Helper columns are highlighted in green and are meant to help you, the developer, and other future developers understand and maintain this document and write tests that align to the requirements. Modify, ignore, or delete as needed</t>
+  </si>
+  <si>
+    <t>Handling Compound Requirements</t>
+  </si>
+  <si>
+    <t>Removing Requirements</t>
+  </si>
+  <si>
+    <t>If after release of the requirements artifact, if a requirement must be removed for some reason, its ID must be retired. To remove a requirement and indicate that the ID is retired, set the Conformance column to DEPRECATED. Note that release may include the start of development of a test kit where requirement IDs have been mapped to tests as ensuring they are up to date with respect to the new requirement Ids may be tricky.</t>
+  </si>
+  <si>
+    <t>Many statements in IGs are compound requirements: they contain multiple requirements in a single context.
+Below is an example of splitting up a compound requirement:
+Original text: The ice cream parlor SHALL sell ice cream in waffle cones and offer chocolate sprinkle toppings.
+Requirements:
+1. The ice cream parlor SHALL sell icecream in waffle cones.
+2. The ice cream parlor SHALL... offer chocolate sprinkle toppings.</t>
+  </si>
+  <si>
+    <t>Requirements get rendered using markdown (https://www.markdownguide.org/basic-syntax/) when displayed in Inferno. This allows some formatting to maintained by using markdown syntax, including for links (https://www.markdownguide.org/basic-syntax/#links). It is recommended that these details be maintained when possible when capturing requirements.</t>
+  </si>
+  <si>
+    <t>Requirements Formatting</t>
+  </si>
+  <si>
+    <t>Requirements Extraction Best Practices</t>
+  </si>
+  <si>
+    <t>Extracting requirements from a FHIR IG or related regulation can be challenging. The requirements are often in a narrative form, use unclear language, and do not have an associated identifier. The basic process that this spreadsheet supports is to turn the narrative sections of an IG or other narrative requirements source into discrete atomic requirements each with a referenceable identifier. Because the way that requirements are represented in narratives can vary depending on the context and domain, the details of how identify and extract requirements may be different across specifications. This template provides
+- guidance on what information to collect in order to use extracted requirements within Inferno. See the column details described below.
+- best practices for representing requirements. See the Requirements Extraction Best Practices described below.</t>
+  </si>
+  <si>
+    <t>Adding Context and Removing Extra Details</t>
+  </si>
+  <si>
+    <t>Each requirement statement should be stand-alone, meaning it should include enough information to understand it when displayed and read separately. It should also be atomic and concise. This may require the addition or removal of details from the extracted text. To make what has been changed clear, inferno recommends using the following syntax:
+- when adding context or otherwise modifying the text, such as for capitalization, put the added context in square brackets, e.g., "[this is added context to] a requirement".
+- when removing content, use an ellipsis (three periods) to indicate where it was removed, e.g., "Some superflous details were removed ... from the middle of this requirement".
+For example, when extracting requiremenst from the narrative text "The ice cream parlor SHALL sell ice cream in waffle cones. It SHALL also offer chocolate sprinkle toppings.", the "It" in the second sentence cannot stand alone and the word "also" only makes sense in the context of the first sentence, but is not needed if the second is standing alone. One way to represent the second sentence would be add context from the first setence and remove the superflous details using the syntax described above: "[The ice cream parlor] SHALL ...offer chocolate sprinkle toppings."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1549,13 +790,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1576,41 +810,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow (Body)"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow (Body)"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1659,8 +873,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1702,37 +928,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1743,66 +945,8 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1847,72 +991,72 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2249,86 +1393,449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AA7094-ECFF-0B4E-A5C9-6F41B8D76EEB}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="133.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="21"/>
-    <col min="3" max="3" width="91.1640625" style="21" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="16"/>
+    <col min="1" max="1" width="16.33203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="133.5" style="39" customWidth="1"/>
+    <col min="3" max="3" width="52.5" style="39" customWidth="1"/>
+    <col min="4" max="4" width="91.1640625" style="21" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="340" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="B4" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:4" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
-    </row>
-    <row r="3" spans="1:3" ht="134" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="33"/>
-    </row>
-    <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-    </row>
-    <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="33"/>
-    </row>
-    <row r="6" spans="1:3" ht="164" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="B14" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="28"/>
-    </row>
-    <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="41"/>
-    </row>
-    <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
-      <c r="B8" s="42"/>
-    </row>
-    <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
-      <c r="B9" s="37"/>
-    </row>
-    <row r="10" spans="1:3" ht="292" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="B15" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="33" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="B16" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A19" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="22"/>
+    </row>
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="22"/>
+    </row>
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="16"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="16"/>
+    </row>
+    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="16"/>
+    </row>
+    <row r="34" spans="1:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="A34" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="16"/>
+    </row>
+    <row r="35" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="40"/>
+    </row>
+    <row r="36" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="43"/>
+    </row>
+    <row r="37" spans="1:4" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="40"/>
+      <c r="D37" s="16"/>
+    </row>
+    <row r="38" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B8"/>
+  <mergeCells count="17">
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2370,64 +1877,64 @@
   <sheetData>
     <row r="1" spans="1:36" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="U1" s="6"/>
       <c r="Z1" s="6"/>
@@ -2436,34 +1943,34 @@
       <c r="A2" s="7">
         <v>12</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="G2" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M2" s="9" t="str" cm="1">
         <f t="array" ref="M2">PAGE_NAME(B2)</f>
@@ -3477,7 +2984,7 @@
       </c>
     </row>
     <row r="96" spans="6:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="F96" s="30"/>
+      <c r="F96" s="23"/>
       <c r="M96" s="9" t="str" cm="1">
         <f t="array" ref="M96">PAGE_NAME(B96)</f>
         <v/>
@@ -6079,68 +5586,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="43"/>
+      <c r="A1" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:2" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -6167,19 +5674,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -6187,13 +5694,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -6213,67 +5720,67 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -6282,28 +5789,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -6557,26 +6042,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E19681A-8DD3-40CB-9262-8533E89B98A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6594,4 +6082,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>